<commit_message>
PRJ | Export Transaction | Thien
</commit_message>
<xml_diff>
--- a/supplier.xlsx
+++ b/supplier.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thien\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thien\OneDrive\Documents\GitHub\warehouse_project_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2154C96A-47CB-4A12-B9F6-3598DA1059C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66EA203-D3B5-47EA-AC86-98D0648A3ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Address</t>
   </si>
@@ -57,69 +57,6 @@
     <t>email2@example.com</t>
   </si>
   <si>
-    <t>CHI NHANH MIKA</t>
-  </si>
-  <si>
-    <t>CONG TY TNHH BOT NANG TRUNG CHANH</t>
-  </si>
-  <si>
-    <t>CONG TY TNHH SAN XUAT THUONG MAI TIEN HAI</t>
-  </si>
-  <si>
-    <t>CTY CP BETTER RESIN</t>
-  </si>
-  <si>
-    <t>GIA LUONG</t>
-  </si>
-  <si>
-    <t>CTY CP XNK THINH AN</t>
-  </si>
-  <si>
-    <t>CTY TNHH CONNELL BROS. (VIETNAM)</t>
-  </si>
-  <si>
-    <t>DUY THANH</t>
-  </si>
-  <si>
-    <t>CTY TNHH THUONG MAI VA DICH VU HOA CHAT VIET</t>
-  </si>
-  <si>
-    <t>CTY TNHH KIEN VUONG</t>
-  </si>
-  <si>
-    <t>vend-01</t>
-  </si>
-  <si>
-    <t>vend-02</t>
-  </si>
-  <si>
-    <t>vend-03</t>
-  </si>
-  <si>
-    <t>vend-04</t>
-  </si>
-  <si>
-    <t>vend-05</t>
-  </si>
-  <si>
-    <t>vend-06</t>
-  </si>
-  <si>
-    <t>vend-08</t>
-  </si>
-  <si>
-    <t>vend-09</t>
-  </si>
-  <si>
-    <t>vend-07</t>
-  </si>
-  <si>
-    <t>vend-00</t>
-  </si>
-  <si>
-    <t>CHI NHANH MIKA1</t>
-  </si>
-  <si>
     <t>Sup_code</t>
   </si>
   <si>
@@ -130,6 +67,99 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>sup-01</t>
+  </si>
+  <si>
+    <t>sup-02</t>
+  </si>
+  <si>
+    <t>sup-03</t>
+  </si>
+  <si>
+    <t>sup-04</t>
+  </si>
+  <si>
+    <t>sup-05</t>
+  </si>
+  <si>
+    <t>sup-06</t>
+  </si>
+  <si>
+    <t>sup-07</t>
+  </si>
+  <si>
+    <t>sup-08</t>
+  </si>
+  <si>
+    <t>sup-09</t>
+  </si>
+  <si>
+    <t>sup-10</t>
+  </si>
+  <si>
+    <t>email3@example.com</t>
+  </si>
+  <si>
+    <t>0302226413</t>
+  </si>
+  <si>
+    <t>0302226414</t>
+  </si>
+  <si>
+    <t>0302226415</t>
+  </si>
+  <si>
+    <t>0302226416</t>
+  </si>
+  <si>
+    <t>0302226417</t>
+  </si>
+  <si>
+    <t>0302226418</t>
+  </si>
+  <si>
+    <t>0302226419</t>
+  </si>
+  <si>
+    <t>0302226420</t>
+  </si>
+  <si>
+    <t>0302226421</t>
+  </si>
+  <si>
+    <t>Something Street</t>
+  </si>
+  <si>
+    <t>Kinh Do 1</t>
+  </si>
+  <si>
+    <t>Kinh Do 2</t>
+  </si>
+  <si>
+    <t>Kinh Do 3</t>
+  </si>
+  <si>
+    <t>Kinh Do 4</t>
+  </si>
+  <si>
+    <t>ChinSu 1</t>
+  </si>
+  <si>
+    <t>ChinSu 2</t>
+  </si>
+  <si>
+    <t>ChinSu 3</t>
+  </si>
+  <si>
+    <t>ChinSu 4</t>
+  </si>
+  <si>
+    <t>ChinSu 5</t>
+  </si>
+  <si>
+    <t>ChinSu 6</t>
   </si>
 </sst>
 </file>
@@ -140,7 +170,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00;\-"/>
     <numFmt numFmtId="165" formatCode="#,##0;\-#,##0;\-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -183,12 +213,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
     </font>
   </fonts>
   <fills count="4">
@@ -243,7 +267,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -272,15 +296,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
@@ -699,15 +714,15 @@
   </sheetPr>
   <dimension ref="A1:G1100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.88671875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
@@ -716,16 +731,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -734,18 +749,18 @@
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>5</v>
@@ -756,169 +771,223 @@
       <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="b">
+      <c r="G2" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>16</v>
+      <c r="A3" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="13" t="b">
+        <v>32</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>17</v>
+      <c r="A4" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="13" t="b">
+        <v>30</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>18</v>
+      <c r="A5" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="13" t="b">
+        <v>30</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>19</v>
+      <c r="A6" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="13" t="b">
+        <v>35</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="13" t="b">
+      <c r="E7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
+      <c r="A8" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="13" t="b">
+        <v>30</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
+      <c r="A9" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="13" t="b">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>22</v>
+      <c r="A10" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="13" t="b">
+        <v>39</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>23</v>
+      <c r="A11" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="13" t="b">
+        <v>30</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
@@ -985,15 +1054,24 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="A2:G12" xr:uid="{2680481B-0139-4802-867F-3883BB61A5B2}"/>
+      <autoFilter ref="A2:G12" xr:uid="{E56E2B1B-7256-48F9-89A2-F93756036A5A}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{8EF72F93-3BB0-4D74-83BF-730FBB71E41E}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{87298097-9E9F-4BB5-B1A8-B6A93824D42C}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{D0582EC0-2A14-4657-A5B4-A96660746563}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{FE5423DA-FD27-4C5D-9970-C9C2442E18DE}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{445E38A5-35CF-434C-A1EF-6B561EB99FD2}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{58E6F1AE-09E0-4E18-9383-CA49DEFD637C}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{E9241758-6B0C-4ED8-80BB-CE8CCDB738CD}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{E7755BFF-3256-425A-98A5-5C5DB24C8058}"/>
+    <hyperlink ref="D9" r:id="rId10" xr:uid="{4D4DD1D8-F846-44D6-8617-5D821F4714E7}"/>
+    <hyperlink ref="D11" r:id="rId11" xr:uid="{925B5C8B-B8EF-43C3-823D-2A9E21F33A8A}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId12"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>